<commit_message>
Revert "updating testcase of adding 20 items into cart"
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/ALL_PAGES/END_TO_END/TC40_Adding_MultipleItems_QuickOrder.xlsx
+++ b/Input_files/Actual_testcases/Kaman/ALL_PAGES/END_TO_END/TC40_Adding_MultipleItems_QuickOrder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KamanProd_ChangeBranch\Kaman_Production_Sanity\Input_files\Actual_testcases\Kaman\ALL_PAGES\END_TO_END\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A91B94F-8B60-4E86-82E9-24E1E155BBA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7643D8E1-73F2-48A7-847C-7295A7677E85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TC40_Adding_MultipleItems_Quick" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="67">
   <si>
     <t>TestCase</t>
   </si>
@@ -672,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37:E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -798,63 +798,61 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="B9" s="7" t="s">
+      <c r="A9" s="7"/>
+      <c r="B9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="B10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="3"/>
-      <c r="B10" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1">
+      <c r="D10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="3"/>
       <c r="B11" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
       <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1">
       <c r="A12" s="3"/>
-      <c r="B12" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="B12" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1">
       <c r="A13" s="3"/>
       <c r="B13" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="7" t="s">
+      <c r="C13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -863,13 +861,13 @@
         <v>13</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -878,13 +876,13 @@
         <v>13</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -893,13 +891,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -908,13 +906,13 @@
         <v>13</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -923,13 +921,13 @@
         <v>13</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -938,13 +936,13 @@
         <v>13</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -953,13 +951,13 @@
         <v>13</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -968,13 +966,13 @@
         <v>13</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -983,13 +981,13 @@
         <v>13</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -998,13 +996,13 @@
         <v>13</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1013,13 +1011,13 @@
         <v>13</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1028,13 +1026,13 @@
         <v>13</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1043,13 +1041,13 @@
         <v>13</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1058,13 +1056,13 @@
         <v>13</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1073,13 +1071,13 @@
         <v>13</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1088,13 +1086,13 @@
         <v>13</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1103,13 +1101,13 @@
         <v>13</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1118,71 +1116,71 @@
         <v>13</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="3"/>
-      <c r="B32" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" s="3"/>
+      <c r="B32" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="3"/>
-      <c r="B33" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>12</v>
+      <c r="B33" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="E33" s="3"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="3"/>
-      <c r="B34" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C34" s="8"/>
-      <c r="D34" s="3"/>
+      <c r="B34" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="E34" s="3"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="3"/>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="8"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="3"/>
+      <c r="B36" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C36" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E35" s="3"/>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="7"/>
-      <c r="B36" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>64</v>
-      </c>
       <c r="D36" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E36" s="7" t="s">
-        <v>64</v>
-      </c>
+      <c r="E36" s="3"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="7"/>
@@ -1190,40 +1188,55 @@
         <v>57</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="7"/>
       <c r="B38" s="8" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E38" s="7"/>
+      <c r="E38" s="7" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="7"/>
       <c r="B39" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E39" s="7"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="7"/>
+      <c r="B40" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="D39" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E39" s="7"/>
+      <c r="D40" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
@@ -1236,8 +1249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B60"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1604,6 +1617,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100599AB90ED4ADBD46B68D7A0832AE2D34" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4d93929aa8d4e603f371af1ff5e0b517">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e6243fcc-5e87-4459-985d-7491a55b4be2" xmlns:ns3="904b644c-3cf7-40e5-b5a5-e101a1ff52b5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="17e9716027504630c423500e26042861" ns2:_="" ns3:_="">
     <xsd:import namespace="e6243fcc-5e87-4459-985d-7491a55b4be2"/>
@@ -1814,22 +1842,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="904b644c-3cf7-40e5-b5a5-e101a1ff52b5"/>
+    <ds:schemaRef ds:uri="e6243fcc-5e87-4459-985d-7491a55b4be2"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CAE325E-5F3B-4FE5-B026-F899F4FA3755}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1846,29 +1884,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="904b644c-3cf7-40e5-b5a5-e101a1ff52b5"/>
-    <ds:schemaRef ds:uri="e6243fcc-5e87-4459-985d-7491a55b4be2"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>